<commit_message>
pet_hotel befoure it's move
</commit_message>
<xml_diff>
--- a/app/PetHotel/OwnersReport.xlsx
+++ b/app/PetHotel/OwnersReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="449" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="240" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,9 +17,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Platypus report layout template</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>E-mail</t>
   </si>
   <si>
     <t>${model.ownersQuery.fullName}</t>
@@ -157,17 +172,18 @@
   <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50607287449393"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3724696356275"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1174089068826"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2267206477733"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50607287449393"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9068825910931"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3967611336032"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.080971659919"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6153846153846"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50607287449393"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -188,21 +204,38 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>